<commit_message>
updated code with new
</commit_message>
<xml_diff>
--- a/Data/NIFTY50.xlsx
+++ b/Data/NIFTY50.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,771 +476,841 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45350</v>
+        <v>45352</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>22086.35</t>
+          <t>22116.30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>22221.30</t>
+          <t>22061.60</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>22228.45</t>
+          <t>22131.50</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>22022.75</t>
+          <t>22061.60</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>75.70K</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-0.50%</t>
+          <t>0.37%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45349</v>
+        <v>45323</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>22198.35</t>
+          <t>22034.10</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>22090.20</t>
+          <t>21774.05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>22218.25</t>
+          <t>22293.20</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>22085.65</t>
+          <t>21531.90</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>252.20B</t>
+          <t>6368.00B</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.34%</t>
+          <t>1.42%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45348</v>
+        <v>45292</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>22122.05</t>
+          <t>21725.70</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>22169.20</t>
+          <t>21727.75</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>22202.15</t>
+          <t>22124.15</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>22075.15</t>
+          <t>21137.20</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>207.78B</t>
+          <t>6824.38B</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-0.41%</t>
+          <t>-0.03%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45345</v>
+        <v>45261</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>22212.70</t>
+          <t>21731.40</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>22290.00</t>
+          <t>20194.10</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>22297.50</t>
+          <t>21801.45</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>22186.10</t>
+          <t>20183.70</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>225.98B</t>
+          <t>6121.37B</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-0.02%</t>
+          <t>7.94%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45344</v>
+        <v>45231</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>22217.45</t>
+          <t>20133.15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>22081.55</t>
+          <t>19064.05</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>22252.50</t>
+          <t>20158.70</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>21875.25</t>
+          <t>18973.70</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>343.50B</t>
+          <t>4423.32B</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.74%</t>
+          <t>5.52%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45343</v>
+        <v>45200</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>22055.05</t>
+          <t>19079.60</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>22248.85</t>
+          <t>19622.40</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>22249.40</t>
+          <t>19849.75</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>21997.95</t>
+          <t>18837.85</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>364.55B</t>
+          <t>4248.51B</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>-0.64%</t>
+          <t>-2.84%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45342</v>
+        <v>45170</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>22196.95</t>
+          <t>19638.30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>22099.20</t>
+          <t>19258.15</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>22215.60</t>
+          <t>20222.45</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>22045.85</t>
+          <t>19255.70</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>295.71B</t>
+          <t>5666.41B</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.34%</t>
+          <t>2.00%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45341</v>
+        <v>45139</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>22122.25</t>
+          <t>19253.80</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>22103.45</t>
+          <t>19784.00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>22186.65</t>
+          <t>19795.60</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>22021.05</t>
+          <t>19223.65</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6253.99B</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.37%</t>
+          <t>-2.53%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45338</v>
+        <v>45108</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>22040.70</t>
+          <t>19753.80</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>22020.30</t>
+          <t>19246.50</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>22068.65</t>
+          <t>19991.85</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>21968.95</t>
+          <t>19234.40</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>343.89B</t>
+          <t>5802.27B</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.59%</t>
+          <t>2.94%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45337</v>
+        <v>45078</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21910.75</t>
+          <t>19189.05</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>21906.55</t>
+          <t>18579.40</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>21953.85</t>
+          <t>19201.70</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>21794.80</t>
+          <t>18464.55</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>345.39B</t>
+          <t>5144.19B</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.32%</t>
+          <t>3.53%</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45336</v>
+        <v>45047</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21840.05</t>
+          <t>18534.40</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>21578.15</t>
+          <t>18124.80</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>21870.85</t>
+          <t>18662.45</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>21530.20</t>
+          <t>18042.40</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>359.12B</t>
+          <t>5737.40B</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0.45%</t>
+          <t>2.60%</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45335</v>
+        <v>45017</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21743.25</t>
+          <t>18065.00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>21664.30</t>
+          <t>17427.95</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>21766.80</t>
+          <t>18089.15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>21543.35</t>
+          <t>17312.75</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>365.79B</t>
+          <t>4459.76B</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0.59%</t>
+          <t>4.06%</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45334</v>
+        <v>44986</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21616.05</t>
+          <t>17359.75</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>21800.80</t>
+          <t>17360.10</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>21831.70</t>
+          <t>17799.95</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>21574.75</t>
+          <t>16828.35</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>287.44B</t>
+          <t>5622.28B</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>-0.76%</t>
+          <t>0.32%</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45331</v>
+        <v>44958</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21782.50</t>
+          <t>17303.95</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>21727.00</t>
+          <t>17811.60</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>21804.45</t>
+          <t>18134.75</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>21629.90</t>
+          <t>17255.20</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>349.22B</t>
+          <t>5685.63B</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0.30%</t>
+          <t>-2.03%</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45330</v>
+        <v>44927</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>21717.95</t>
+          <t>17662.15</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>22009.65</t>
+          <t>18131.70</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22011.05</t>
+          <t>18251.95</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>21665.30</t>
+          <t>17405.55</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>491.07B</t>
+          <t>5632.81B</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>-0.97%</t>
+          <t>-2.45%</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45329</v>
+        <v>44896</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>21930.50</t>
+          <t>18105.30</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>22045.05</t>
+          <t>18871.95</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>22053.30</t>
+          <t>18887.60</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>21860.15</t>
+          <t>17774.25</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>346.26B</t>
+          <t>4741.44B</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.01%</t>
+          <t>-3.48%</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45328</v>
+        <v>44866</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21929.40</t>
+          <t>18758.35</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>21825.20</t>
+          <t>18130.70</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>21951.40</t>
+          <t>18816.05</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>21737.55</t>
+          <t>17959.20</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>370.97B</t>
+          <t>5257.00B</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.72%</t>
+          <t>4.14%</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45327</v>
+        <v>44835</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>21771.70</t>
+          <t>18012.20</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>21921.05</t>
+          <t>17102.10</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>21964.30</t>
+          <t>18022.80</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>21726.95</t>
+          <t>16855.55</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>440.85B</t>
+          <t>4539.96B</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>-0.38%</t>
+          <t>5.37%</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45324</v>
+        <v>44805</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>21853.80</t>
+          <t>17094.35</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>21812.75</t>
+          <t>17485.70</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>22126.80</t>
+          <t>18096.15</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>21805.55</t>
+          <t>16747.70</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>442.79B</t>
+          <t>6896.51B</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0.72%</t>
+          <t>-3.74%</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45323</v>
+        <v>44774</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21697.45</t>
+          <t>17759.30</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>21780.65</t>
+          <t>17243.20</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>21832.95</t>
+          <t>17992.20</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>21658.75</t>
+          <t>17154.80</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>332.54B</t>
+          <t>5589.51B</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>-0.13%</t>
+          <t>3.50%</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45322</v>
+        <v>44743</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21725.70</t>
+          <t>17158.25</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>21487.25</t>
+          <t>15703.70</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>21741.35</t>
+          <t>17172.80</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>21448.85</t>
+          <t>15511.05</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>410.58B</t>
+          <t>5475.27B</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0.95%</t>
+          <t>8.73%</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45321</v>
+        <v>44713</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21522.10</t>
+          <t>15780.25</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>21775.75</t>
+          <t>16594.40</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>21813.05</t>
+          <t>16793.85</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>21501.80</t>
+          <t>15183.40</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>375.14B</t>
+          <t>5514.20B</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>-0.99%</t>
+          <t>-4.85%</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>44682</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>16584.55</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>16924.45</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>17132.85</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>15735.75</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>6343.31B</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-3.03%</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>44652</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>17102.55</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>17436.90</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>18114.65</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>16824.70</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>5658.25B</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>-2.07%</t>
         </is>
       </c>
     </row>

</xml_diff>